<commit_message>
minor changes to model
</commit_message>
<xml_diff>
--- a/20191204_Parts_to_order.xlsx
+++ b/20191204_Parts_to_order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niklas\Documents\StArb_Mars_Rover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niklas\Documents\01_DHBW\StArb_Mars_Rover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F707052D-F141-4E79-BD31-675F401BDDDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CA9E5D-DDAB-4F80-97BE-F279D6CE032E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17145" yWindow="13140" windowWidth="17355" windowHeight="7875" xr2:uid="{C9532969-CDFC-43B5-9DFA-984D407C82C5}"/>
+    <workbookView xWindow="390" yWindow="990" windowWidth="21600" windowHeight="11385" xr2:uid="{C9532969-CDFC-43B5-9DFA-984D407C82C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>x12</t>
   </si>
@@ -63,9 +63,6 @@
     <t>3492c01</t>
   </si>
   <si>
-    <t>Gray</t>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
@@ -73,6 +70,12 @@
   </si>
   <si>
     <t>Yellow</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Grey</t>
   </si>
 </sst>
 </file>
@@ -132,18 +135,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0470130C-4CA3-419B-B940-3B5F2C0C4835}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,20 +483,20 @@
     <col min="6" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -498,13 +507,13 @@
       <c r="B2" s="5">
         <v>33176</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -513,13 +522,13 @@
         <v>3755</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="6">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -528,13 +537,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -543,13 +552,13 @@
         <v>3613</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -558,13 +567,13 @@
         <v>4730</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="6">
         <v>4</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -573,13 +582,13 @@
         <v>4873</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -588,13 +597,13 @@
         <v>6048</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -605,13 +614,13 @@
       <c r="B9" s="4">
         <v>4033</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -620,13 +629,13 @@
         <v>75535</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="6">
         <v>20</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -637,28 +646,79 @@
       <c r="B11" s="4">
         <v>3245</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="6">
         <v>4</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>7</v>
+      <c r="E11" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>2569</v>
+      </c>
+      <c r="B13" s="7">
+        <v>4251564</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>6111</v>
+      </c>
+      <c r="B14" s="7">
+        <v>611101</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="6">
+        <v>10</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>330701</v>
+      </c>
+      <c r="B15" s="7">
+        <v>3307</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="6">
+        <v>3</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>